<commit_message>
Addet modified file Ukrposhta.xlsx
</commit_message>
<xml_diff>
--- a/Ukrposhta.xlsx
+++ b/Ukrposhta.xlsx
@@ -1239,10 +1239,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1257,6 +1263,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1276,22 +1285,13 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1434,17 +1434,6 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="uk-UA" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Nokia</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Lumia 535 Windows 10 Mobail </a:t>
-          </a:r>
-          <a:endParaRPr lang="uk-UA" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="uk-UA" sz="1100"/>
@@ -2207,7 +2196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:E6"/>
     </sheetView>
   </sheetViews>
@@ -2219,120 +2208,120 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="40"/>
     </row>
     <row r="5" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="40"/>
     </row>
     <row r="6" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="40"/>
     </row>
     <row r="10" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="40"/>
     </row>
     <row r="11" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="40"/>
     </row>
     <row r="12" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="40"/>
     </row>
     <row r="13" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="40"/>
     </row>
     <row r="17" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="44" t="s">
         <v>226</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="40"/>
       <c r="G17" s="40"/>
     </row>
     <row r="18" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
     </row>
     <row r="20" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="40"/>
       <c r="G20" s="40"/>
     </row>
     <row r="24" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="40"/>
     </row>
     <row r="25" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="40"/>
     </row>
     <row r="26" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="40"/>
     </row>
     <row r="27" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="40"/>
     </row>
   </sheetData>
@@ -2368,10 +2357,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="34" t="s">
@@ -2380,23 +2369,23 @@
       <c r="C4" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
     </row>
     <row r="7" spans="2:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
@@ -2455,10 +2444,10 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="48"/>
     </row>
     <row r="15" spans="2:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="34" t="s">
@@ -2477,16 +2466,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="48"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="49" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2494,7 +2483,7 @@
       <c r="B19" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="50"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="34">
@@ -2584,7 +2573,7 @@
       <c r="B32" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="46" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2592,13 +2581,13 @@
       <c r="B33" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="44"/>
+      <c r="C33" s="46"/>
     </row>
     <row r="34" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B34" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="46" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2606,38 +2595,38 @@
       <c r="B35" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="44"/>
+      <c r="C35" s="46"/>
     </row>
     <row r="36" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="44"/>
+      <c r="C36" s="46"/>
     </row>
     <row r="37" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="44"/>
+      <c r="C37" s="46"/>
     </row>
     <row r="38" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B38" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="44"/>
+      <c r="C38" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C18:C19"/>
   </mergeCells>
   <hyperlinks>
@@ -2659,14 +2648,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P4" s="57" t="s">
+      <c r="P4" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="Q4" s="57"/>
+      <c r="Q4" s="60"/>
     </row>
     <row r="5" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2684,7 +2673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2768,7 +2759,7 @@
       </c>
       <c r="E8" s="6"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="42" t="s">
         <v>239</v>
       </c>
       <c r="J8" s="38"/>
@@ -3284,14 +3275,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K6" s="56" t="s">
+      <c r="K6" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="L6" s="56"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3320,10 +3311,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -3334,23 +3325,23 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="H5" s="56"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="38"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="38"/>
     </row>
     <row r="7" spans="2:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3410,10 +3401,10 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="48"/>
     </row>
     <row r="15" spans="2:9" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -3432,16 +3423,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="48"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="49" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3449,7 +3440,7 @@
       <c r="B19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="50"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
@@ -3487,7 +3478,7 @@
       <c r="B24" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="46" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3495,13 +3486,13 @@
       <c r="B25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="44"/>
+      <c r="C25" s="46"/>
     </row>
     <row r="26" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3509,38 +3500,38 @@
       <c r="B27" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="46"/>
     </row>
     <row r="28" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="44"/>
+      <c r="C28" s="46"/>
     </row>
     <row r="29" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="44"/>
+      <c r="C29" s="46"/>
     </row>
     <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="G5:H6"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C18:C19"/>
   </mergeCells>
   <hyperlinks>
@@ -3573,120 +3564,120 @@
       <c r="A3" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="H3" s="58" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="H3" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="52"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="27" t="s">
         <v>109</v>
       </c>
@@ -3898,25 +3889,25 @@
       <c r="A24" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="52">
         <v>45023</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
@@ -3930,109 +3921,109 @@
       <c r="A29" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F36" s="52"/>
+      <c r="F36" s="55"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="27" t="s">
         <v>109</v>
       </c>
@@ -4117,25 +4108,25 @@
       <c r="A42" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="49">
+      <c r="B42" s="52">
         <v>45023</v>
       </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
@@ -4149,109 +4140,109 @@
       <c r="A48" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="C49" s="54"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="51" t="s">
+      <c r="B51" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="51" t="s">
+      <c r="B52" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="51" t="s">
+      <c r="B53" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="54"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="51" t="s">
+      <c r="B54" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="52" t="s">
+      <c r="A55" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="52" t="s">
+      <c r="B55" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="52" t="s">
+      <c r="C55" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="52" t="s">
+      <c r="D55" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E55" s="52" t="s">
+      <c r="E55" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F55" s="52"/>
+      <c r="F55" s="55"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
-      <c r="B56" s="52"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
+      <c r="A56" s="55"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
       <c r="E56" s="27" t="s">
         <v>109</v>
       </c>
@@ -4352,25 +4343,25 @@
       <c r="A62" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B62" s="49">
+      <c r="B62" s="52">
         <v>45023</v>
       </c>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="50" t="s">
+      <c r="B63" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
@@ -4384,109 +4375,109 @@
       <c r="A68" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="53" t="s">
+      <c r="B68" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="53"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="53"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="57"/>
+      <c r="F69" s="57"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B70" s="51" t="s">
+      <c r="B70" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="51"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="51"/>
-      <c r="F70" s="51"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="54"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="51" t="s">
+      <c r="B71" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="51"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
-      <c r="F71" s="51"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B72" s="51" t="s">
+      <c r="B72" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="51"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="51" t="s">
+      <c r="B73" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="51"/>
-      <c r="F73" s="51"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B74" s="51" t="s">
+      <c r="B74" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-      <c r="F74" s="51"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="54"/>
+      <c r="E74" s="54"/>
+      <c r="F74" s="54"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="52" t="s">
+      <c r="A75" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B75" s="52" t="s">
+      <c r="B75" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C75" s="52" t="s">
+      <c r="C75" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D75" s="52" t="s">
+      <c r="D75" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E75" s="52" t="s">
+      <c r="E75" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F75" s="52"/>
+      <c r="F75" s="55"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="52"/>
-      <c r="B76" s="52"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="52"/>
+      <c r="A76" s="55"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
       <c r="E76" s="27" t="s">
         <v>109</v>
       </c>
@@ -4682,25 +4673,25 @@
       <c r="A88" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B88" s="49">
+      <c r="B88" s="52">
         <v>45023</v>
       </c>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-      <c r="E88" s="50"/>
-      <c r="F88" s="50"/>
+      <c r="C88" s="53"/>
+      <c r="D88" s="53"/>
+      <c r="E88" s="53"/>
+      <c r="F88" s="53"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B89" s="50" t="s">
+      <c r="B89" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="50"/>
+      <c r="C89" s="53"/>
+      <c r="D89" s="53"/>
+      <c r="E89" s="53"/>
+      <c r="F89" s="53"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="19"/>
@@ -4714,109 +4705,109 @@
       <c r="A94" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="53" t="s">
+      <c r="B94" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C94" s="53"/>
-      <c r="D94" s="53"/>
-      <c r="E94" s="53"/>
-      <c r="F94" s="53"/>
+      <c r="C94" s="56"/>
+      <c r="D94" s="56"/>
+      <c r="E94" s="56"/>
+      <c r="F94" s="56"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="54" t="s">
+      <c r="B95" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="C95" s="54"/>
-      <c r="D95" s="54"/>
-      <c r="E95" s="54"/>
-      <c r="F95" s="54"/>
+      <c r="C95" s="57"/>
+      <c r="D95" s="57"/>
+      <c r="E95" s="57"/>
+      <c r="F95" s="57"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="51" t="s">
+      <c r="B96" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C96" s="51"/>
-      <c r="D96" s="51"/>
-      <c r="E96" s="51"/>
-      <c r="F96" s="51"/>
+      <c r="C96" s="54"/>
+      <c r="D96" s="54"/>
+      <c r="E96" s="54"/>
+      <c r="F96" s="54"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="51" t="s">
+      <c r="B97" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C97" s="51"/>
-      <c r="D97" s="51"/>
-      <c r="E97" s="51"/>
-      <c r="F97" s="51"/>
+      <c r="C97" s="54"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="54"/>
+      <c r="F97" s="54"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B98" s="51" t="s">
+      <c r="B98" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C98" s="51"/>
-      <c r="D98" s="51"/>
-      <c r="E98" s="51"/>
-      <c r="F98" s="51"/>
+      <c r="C98" s="54"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="54"/>
+      <c r="F98" s="54"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B99" s="51" t="s">
+      <c r="B99" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="51"/>
-      <c r="D99" s="51"/>
-      <c r="E99" s="51"/>
-      <c r="F99" s="51"/>
+      <c r="C99" s="54"/>
+      <c r="D99" s="54"/>
+      <c r="E99" s="54"/>
+      <c r="F99" s="54"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B100" s="51" t="s">
+      <c r="B100" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C100" s="51"/>
-      <c r="D100" s="51"/>
-      <c r="E100" s="51"/>
-      <c r="F100" s="51"/>
+      <c r="C100" s="54"/>
+      <c r="D100" s="54"/>
+      <c r="E100" s="54"/>
+      <c r="F100" s="54"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="52" t="s">
+      <c r="A101" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B101" s="52" t="s">
+      <c r="B101" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C101" s="52" t="s">
+      <c r="C101" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D101" s="52" t="s">
+      <c r="D101" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="E101" s="52" t="s">
+      <c r="E101" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F101" s="52"/>
+      <c r="F101" s="55"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="52"/>
-      <c r="B102" s="52"/>
-      <c r="C102" s="52"/>
-      <c r="D102" s="52"/>
+      <c r="A102" s="55"/>
+      <c r="B102" s="55"/>
+      <c r="C102" s="55"/>
+      <c r="D102" s="55"/>
       <c r="E102" s="36" t="s">
         <v>109</v>
       </c>
@@ -5032,28 +5023,83 @@
       <c r="A116" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B116" s="49">
+      <c r="B116" s="52">
         <v>45023</v>
       </c>
-      <c r="C116" s="50"/>
-      <c r="D116" s="50"/>
-      <c r="E116" s="50"/>
-      <c r="F116" s="50"/>
+      <c r="C116" s="53"/>
+      <c r="D116" s="53"/>
+      <c r="E116" s="53"/>
+      <c r="F116" s="53"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="B117" s="50" t="s">
+      <c r="B117" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C117" s="50"/>
-      <c r="D117" s="50"/>
-      <c r="E117" s="50"/>
-      <c r="F117" s="50"/>
+      <c r="C117" s="53"/>
+      <c r="D117" s="53"/>
+      <c r="E117" s="53"/>
+      <c r="F117" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:F75"/>
     <mergeCell ref="H3:J5"/>
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B89:F89"/>
@@ -5061,11 +5107,6 @@
     <mergeCell ref="B72:F72"/>
     <mergeCell ref="B73:F73"/>
     <mergeCell ref="B74:F74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:F75"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B63:F63"/>
     <mergeCell ref="B68:F68"/>
@@ -5075,56 +5116,6 @@
     <mergeCell ref="B52:F52"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B54:F54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="E101:F101"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F41" location="'Bug report 2'!A1" display="Bug report 2"/>
@@ -5151,10 +5142,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="44"/>
+      <c r="C4" s="46"/>
     </row>
     <row r="5" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -5163,24 +5154,24 @@
       <c r="C5" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="47" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
     </row>
     <row r="8" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
@@ -5239,10 +5230,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="46"/>
+      <c r="C15" s="48"/>
     </row>
     <row r="16" spans="2:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
@@ -5261,16 +5252,16 @@
       </c>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="48"/>
     </row>
     <row r="19" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="49" t="s">
         <v>154</v>
       </c>
     </row>
@@ -5278,7 +5269,7 @@
       <c r="B20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="48"/>
+      <c r="C20" s="50"/>
     </row>
     <row r="21" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
@@ -5316,7 +5307,7 @@
       <c r="B25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="46" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5324,13 +5315,13 @@
       <c r="B26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="44"/>
+      <c r="C26" s="46"/>
     </row>
     <row r="27" spans="2:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="46" t="s">
         <v>148</v>
       </c>
     </row>
@@ -5338,38 +5329,38 @@
       <c r="B28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="44"/>
+      <c r="C28" s="46"/>
     </row>
     <row r="29" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="44"/>
+      <c r="C29" s="46"/>
     </row>
     <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="46"/>
     </row>
     <row r="31" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="44"/>
+      <c r="C31" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="E5:H5"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B18:C18"/>
     <mergeCell ref="C19:C20"/>
   </mergeCells>
   <hyperlinks>
@@ -5395,10 +5386,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -5407,23 +5398,23 @@
       <c r="C4" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
     </row>
     <row r="7" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -5482,10 +5473,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="48"/>
     </row>
     <row r="15" spans="2:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -5504,16 +5495,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="48"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="49" t="s">
         <v>159</v>
       </c>
     </row>
@@ -5521,7 +5512,7 @@
       <c r="B19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="50"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
@@ -5559,7 +5550,7 @@
       <c r="B24" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="46" t="s">
         <v>162</v>
       </c>
     </row>
@@ -5567,13 +5558,13 @@
       <c r="B25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="44"/>
+      <c r="C25" s="46"/>
     </row>
     <row r="26" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="46" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5581,38 +5572,38 @@
       <c r="B27" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="46"/>
     </row>
     <row r="28" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="44"/>
+      <c r="C28" s="46"/>
     </row>
     <row r="29" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="44"/>
+      <c r="C29" s="46"/>
     </row>
     <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C18:C19"/>
   </mergeCells>
   <hyperlinks>
@@ -5640,10 +5631,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -5652,23 +5643,23 @@
       <c r="C4" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
     </row>
     <row r="7" spans="2:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -5727,10 +5718,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="48"/>
     </row>
     <row r="15" spans="2:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -5749,16 +5740,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="48"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="49" t="s">
         <v>159</v>
       </c>
     </row>
@@ -5766,7 +5757,7 @@
       <c r="B19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="50"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
@@ -5864,7 +5855,7 @@
       <c r="B32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="46" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5872,13 +5863,13 @@
       <c r="B33" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="44"/>
+      <c r="C33" s="46"/>
     </row>
     <row r="34" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="46" t="s">
         <v>185</v>
       </c>
     </row>
@@ -5886,38 +5877,38 @@
       <c r="B35" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="44"/>
+      <c r="C35" s="46"/>
     </row>
     <row r="36" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="44"/>
+      <c r="C36" s="46"/>
     </row>
     <row r="37" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="44"/>
+      <c r="C37" s="46"/>
     </row>
     <row r="38" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="44"/>
+      <c r="C38" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C18:C19"/>
   </mergeCells>
   <hyperlinks>
@@ -5948,117 +5939,117 @@
       <c r="B3" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="57" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="I4" s="57" t="s">
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="I4" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
       <c r="F11" s="36" t="s">
         <v>109</v>
       </c>
@@ -6218,133 +6209,133 @@
       <c r="B24" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="52">
         <v>45023</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="57" t="s">
         <v>224</v>
       </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="51" t="s">
+      <c r="C33" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="51" t="s">
+      <c r="C35" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
     </row>
     <row r="36" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="52" t="s">
+      <c r="E36" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="F36" s="52" t="s">
+      <c r="F36" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="55"/>
     </row>
     <row r="37" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="36" t="s">
         <v>109</v>
       </c>
@@ -6526,35 +6517,38 @@
       <c r="B50" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="C50" s="49">
+      <c r="C50" s="52">
         <v>45023</v>
       </c>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="50" t="s">
+      <c r="C51" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="I4:K5"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:G36"/>
     <mergeCell ref="C32:G32"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="B10:B11"/>
@@ -6567,16 +6561,13 @@
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="C31:G31"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" location="'Bug report 5'!A1" display="Bug report 5"/>

</xml_diff>